<commit_message>
updated all copy, fixed css issues to make pages more uniform
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madelinescomputer/Dropbox/MSI/Current Projects/Mapping Project/3 - Mapping Results/2016-09 Data Visualization/For Ben/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bisaacs/projects/msi-map-microsite/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -716,31 +716,19 @@
     <t>No*</t>
   </si>
   <si>
-    <t>Alliance for Water Stewardship*</t>
-  </si>
-  <si>
     <t>Website</t>
   </si>
   <si>
-    <t>Better Biomass*</t>
-  </si>
-  <si>
     <t>Yes*</t>
   </si>
   <si>
     <t>External Complaints Mechanisms</t>
   </si>
   <si>
-    <t xml:space="preserve">Rainforest Alliance* </t>
-  </si>
-  <si>
     <t>Civil Society (5), Other (1)</t>
   </si>
   <si>
     <t>Human Rights/Enviro Law Reference</t>
-  </si>
-  <si>
-    <t>Green-e*</t>
   </si>
   <si>
     <r>
@@ -784,6 +772,18 @@
   </si>
   <si>
     <t xml:space="preserve">Government (2), Industry (3), Civil Society (4), Other (1) </t>
+  </si>
+  <si>
+    <t>Rainforest Alliance</t>
+  </si>
+  <si>
+    <t>Alliance for Water Stewardship</t>
+  </si>
+  <si>
+    <t>Better Biomass</t>
+  </si>
+  <si>
+    <t>Green-e</t>
   </si>
 </sst>
 </file>
@@ -1276,8 +1276,8 @@
   <dimension ref="B1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1299,7 +1299,7 @@
         <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>184</v>
@@ -1320,7 +1320,7 @@
         <v>38</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>39</v>
@@ -1329,7 +1329,7 @@
         <v>40</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>41</v>
@@ -1378,7 +1378,7 @@
     </row>
     <row r="3" spans="2:14" ht="144" x14ac:dyDescent="0.2">
       <c r="B3" s="19" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>138</v>
@@ -1390,7 +1390,7 @@
         <v>134</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G3" s="4">
         <v>2008</v>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="4" spans="2:14" ht="144" x14ac:dyDescent="0.2">
       <c r="B4" s="20" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>139</v>
@@ -1733,10 +1733,10 @@
         <v>42</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="M11" s="10" t="s">
         <v>42</v>
@@ -2128,7 +2128,7 @@
         <v>79</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>80</v>
@@ -2251,7 +2251,7 @@
         <v>85</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G24" s="4">
         <v>2007</v>
@@ -2292,7 +2292,7 @@
         <v>86</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G25" s="4">
         <v>1994</v>
@@ -2321,7 +2321,7 @@
     </row>
     <row r="26" spans="2:14" ht="400" x14ac:dyDescent="0.2">
       <c r="B26" s="20" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>161</v>
@@ -2512,10 +2512,10 @@
         <v>42</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="M30" s="10" t="s">
         <v>43</v>
@@ -2538,7 +2538,7 @@
         <v>96</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G31" s="4">
         <v>2009</v>
@@ -2573,7 +2573,7 @@
         <v>169</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>98</v>
@@ -2731,7 +2731,7 @@
     </row>
     <row r="36" spans="2:14" ht="128" x14ac:dyDescent="0.2">
       <c r="B36" s="20" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>173</v>
@@ -2904,10 +2904,10 @@
         <v>193</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G40" s="4">
         <v>1997</v>

</xml_diff>